<commit_message>
First BIG update : menu and tiles display are on. The MAKEFILE is to do for : main, tilemap & menu.
</commit_message>
<xml_diff>
--- a/ToDoC++.xlsx
+++ b/ToDoC++.xlsx
@@ -166,17 +166,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,226 +481,226 @@
   <dimension ref="B2:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
       <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="6" t="s">
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="6">
+      <c r="H6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="3">
         <f>COUNTIF(F3:F17,"J")</f>
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="3">
         <f>COUNTIF(F3:F17,"S")</f>
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
       <c r="E8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
       <c r="E10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
       <c r="E11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
       <c r="E12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
       <c r="E13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
       <c r="E14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
       <c r="E15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
       <c r="E16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
       <c r="E17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="3" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>